<commit_message>
added customer id for delete
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9480" yWindow="0" windowWidth="27870" windowHeight="12885"/>
+    <workbookView xWindow="10665" yWindow="0" windowWidth="27870" windowHeight="12885"/>
   </bookViews>
   <sheets>
     <sheet name="testData" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
   <si>
     <t>name</t>
   </si>
@@ -67,184 +67,34 @@
     <t>deleteCustomer</t>
   </si>
   <si>
-    <t>cus_GcjlFEiUufsYq9</t>
-  </si>
-  <si>
-    <t>cus_GcjlTIGSiciDgV</t>
-  </si>
-  <si>
-    <t>cus_GcjkQZoUVHI2PG</t>
-  </si>
-  <si>
-    <t>cus_GcjkV7k16XhBUt</t>
-  </si>
-  <si>
-    <t>cus_GcjjOofI12TIt8</t>
-  </si>
-  <si>
-    <t>cus_Gcjj6IR51nWPAT</t>
-  </si>
-  <si>
-    <t>cus_GcjilaP4MoD0Zf</t>
-  </si>
-  <si>
-    <t>cus_Gcji4OuKIU1eww</t>
-  </si>
-  <si>
-    <t>cus_GcjhicS3iHs7uR</t>
-  </si>
-  <si>
-    <t>cus_GcjhFl9iiu1T09</t>
-  </si>
-  <si>
-    <t>cus_Gcjgag86iK1uyt</t>
-  </si>
-  <si>
-    <t>cus_GcjgTfn4wb2Dpf</t>
-  </si>
-  <si>
-    <t>cus_GcjfxB74Mn1dWi</t>
-  </si>
-  <si>
-    <t>cus_Gcjf6B78YY9OmE</t>
-  </si>
-  <si>
-    <t>cus_GcjesVLlKcoMAJ</t>
-  </si>
-  <si>
-    <t>cus_GcjeUe7wGAvvNG</t>
-  </si>
-  <si>
-    <t>cus_GcjdzxxMsNY3FW</t>
-  </si>
-  <si>
-    <t>cus_GcjdxKGoXZP2nl</t>
-  </si>
-  <si>
-    <t>cus_GcjcKULB7fKrjI</t>
-  </si>
-  <si>
-    <t>cus_GcjcFR7PGISiIW</t>
-  </si>
-  <si>
-    <t>cus_GcjbaxHtiKpFYB</t>
-  </si>
-  <si>
-    <t>cus_Gcjbe2BkAuPtcP</t>
-  </si>
-  <si>
-    <t>cus_GcjaUnTdtU117o</t>
-  </si>
-  <si>
-    <t>cus_GcjaT37sU6wGi1</t>
-  </si>
-  <si>
-    <t>cus_GcjZ6xbBnBFKnD</t>
-  </si>
-  <si>
-    <t>cus_GcjZsxLByaQfpz</t>
-  </si>
-  <si>
-    <t>cus_GcjYWbI3QUfBGV</t>
-  </si>
-  <si>
-    <t>cus_GcjYMIPLIc8sOK</t>
-  </si>
-  <si>
-    <t>cus_GcjXiFgFehUTsQ</t>
-  </si>
-  <si>
-    <t>cus_GcjXs1Qvi65wXV</t>
-  </si>
-  <si>
-    <t>cus_GcjWEj5GQjaY4F</t>
-  </si>
-  <si>
-    <t>cus_GcjWIgOAYBw8oy</t>
-  </si>
-  <si>
-    <t>cus_GcjVy0FpWdrRvi</t>
-  </si>
-  <si>
-    <t>cus_GcjVyJwB07e8bi</t>
-  </si>
-  <si>
-    <t>cus_GcjUPvmxjqJMtD</t>
-  </si>
-  <si>
-    <t>cus_GcjUcz5lmCErfe</t>
-  </si>
-  <si>
-    <t>cus_GcjTHYd0IKXBKE</t>
-  </si>
-  <si>
-    <t>cus_GcjTMS1rqtrCTY</t>
-  </si>
-  <si>
-    <t>cus_GcjSA48sj0wohU</t>
-  </si>
-  <si>
-    <t>cus_GcjSJoeziCZyQ0</t>
-  </si>
-  <si>
-    <t>cus_GcjR70kCLBFTiU</t>
-  </si>
-  <si>
-    <t>cus_GcjR69EWPhfCcC</t>
-  </si>
-  <si>
-    <t>cus_GcjQHseen0cq4o</t>
-  </si>
-  <si>
-    <t>cus_GcjQEK0xOW4vD3</t>
-  </si>
-  <si>
-    <t>cus_GcjPAYQst2W7L3</t>
-  </si>
-  <si>
-    <t>cus_GcjPdKxA3PahN5</t>
-  </si>
-  <si>
-    <t>cus_GcjOFeZfsW3FEe</t>
-  </si>
-  <si>
-    <t>cus_GcjOP8IqMeXK5Y</t>
-  </si>
-  <si>
-    <t>cus_GcjN8qKlmJEfn8</t>
-  </si>
-  <si>
-    <t>cus_GcjNtxqsp6tSH4</t>
-  </si>
-  <si>
-    <t>cus_GcjMgo17U4k6K9</t>
-  </si>
-  <si>
-    <t>cus_GcjMHN6jaNCMqI</t>
-  </si>
-  <si>
-    <t>cus_GcjL5ILwhY7wbc</t>
-  </si>
-  <si>
-    <t>cus_GcjLdwHHpHNQTI</t>
-  </si>
-  <si>
-    <t>cus_GcjKoUnQzk24YV</t>
-  </si>
-  <si>
-    <t>cus_GcjK9JbjUDcfGA</t>
-  </si>
-  <si>
-    <t>cus_GcjJplT7RTXlxC</t>
-  </si>
-  <si>
-    <t>cus_GcjJRjWiZdT3VR</t>
-  </si>
-  <si>
-    <t>cus_Gcj0jnTX4syFxH</t>
-  </si>
-  <si>
-    <t>cus_Gcj0mCY4pXiGn4</t>
+    <t>cus_Gck6dcEPDV7X0a</t>
+  </si>
+  <si>
+    <t>cus_Gck6WsSoD0asjT</t>
+  </si>
+  <si>
+    <t>cus_GcjsUGietMXn25</t>
+  </si>
+  <si>
+    <t>cus_GcjsQOkmbA67Cr</t>
+  </si>
+  <si>
+    <t>cus_Gcjrt8qJX0M7Ni</t>
+  </si>
+  <si>
+    <t>cus_GcjrMBC99EdKDY</t>
+  </si>
+  <si>
+    <t>cus_Gcjqc117HUAXzX</t>
+  </si>
+  <si>
+    <t>cus_GcjqALKa0XIrfi</t>
+  </si>
+  <si>
+    <t>cus_GcjpdQGPH3Msof</t>
+  </si>
+  <si>
+    <t>cus_GcjpuocZ6NRUUV</t>
   </si>
 </sst>
 </file>
@@ -573,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:A72"/>
+      <selection activeCell="A13" sqref="A13:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,256 +565,6 @@
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>